<commit_message>
importing selenium webdriver pandas
</commit_message>
<xml_diff>
--- a/Output_Result/test_result/TestResult.xlsx
+++ b/Output_Result/test_result/TestResult.xlsx
@@ -505,14 +505,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>FAIL</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Message: no such element: Unable to locate element: {"method":"xpath","selector":"//button[@id="bubble"]"}
-  (Session info: chrome=91.0.4472.114)
-</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -547,7 +540,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Message: no such element: Unable to locate element: {"method":"xpath","selector":"//h3[contains(text(),'Interested in studying abroad with us?')]"}
+          <t xml:space="preserve">Message: chrome not reachable
   (Session info: chrome=91.0.4472.114)
 </t>
         </is>
@@ -569,7 +562,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Message: no such element: Unable to locate element: {"method":"xpath","selector":"//input[@name='text-765']"}
+          <t xml:space="preserve">Message: chrome not reachable
   (Session info: chrome=91.0.4472.114)
 </t>
         </is>
@@ -591,7 +584,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Message: no such element: Unable to locate element: {"method":"xpath","selector":"//input[@name='email-931']"}
+          <t xml:space="preserve">Message: chrome not reachable
   (Session info: chrome=91.0.4472.114)
 </t>
         </is>
@@ -613,7 +606,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Message: no such element: Unable to locate element: {"method":"xpath","selector":"//input[@name='text-631']"}
+          <t xml:space="preserve">Message: chrome not reachable
   (Session info: chrome=91.0.4472.114)
 </t>
         </is>
@@ -635,7 +628,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Message: no such element: Unable to locate element: {"method":"xpath","selector":"//select[@name='menu-104']"}
+          <t xml:space="preserve">Message: chrome not reachable
   (Session info: chrome=91.0.4472.114)
 </t>
         </is>
@@ -657,7 +650,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Message: no such element: Unable to locate element: {"method":"xpath","selector":"//select[@name='menu-105']"}
+          <t xml:space="preserve">Message: chrome not reachable
   (Session info: chrome=91.0.4472.114)
 </t>
         </is>
@@ -679,7 +672,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Message: no such element: Unable to locate element: {"method":"xpath","selector":"//input[@value='Submit']"}
+          <t xml:space="preserve">Message: chrome not reachable
   (Session info: chrome=91.0.4472.114)
 </t>
         </is>
@@ -701,7 +694,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Message: no such element: Unable to locate element: {"method":"xpath","selector":"//div[@class="wpcf7-response-output"]"}
+          <t xml:space="preserve">Message: chrome not reachable
   (Session info: chrome=91.0.4472.114)
 </t>
         </is>

</xml_diff>

<commit_message>
adding test result and test summary
</commit_message>
<xml_diff>
--- a/Output_Result/test_result/TestResult.xlsx
+++ b/Output_Result/test_result/TestResult.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="TestResults" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="TestSummary" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -671,7 +672,48 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Test Executed On</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>2021-07-03 13:29:51.983579</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Number of Test Cases</t>
+        </is>
+      </c>
+      <c r="B2">
+        <f>(COUNTA(TestResults!A:A) - 1)</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>